<commit_message>
Tesiones en el terreno
</commit_message>
<xml_diff>
--- a/datos_terreno.xlsx
+++ b/datos_terreno.xlsx
@@ -491,10 +491,10 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>18000</v>
@@ -521,10 +521,10 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
-        <v>15.25</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>40000</v>

</xml_diff>

<commit_message>
creacion de tablas en word
</commit_message>
<xml_diff>
--- a/datos_terreno.xlsx
+++ b/datos_terreno.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Espesor [m]</t>
   </si>
@@ -49,7 +49,7 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>c</t>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -57,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,12 +68,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -113,10 +107,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -427,7 +421,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -481,71 +475,104 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>15</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>17</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>12000</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>0.3</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>12</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="1">
         <v>23</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
         <v>0.3</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="1">
         <v>0.49</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="3">
         <v>15</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25000</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
         <v>17.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>18</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>25000</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <v>0.3</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <v>15</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H4" s="1">
         <v>25</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I4" s="1">
         <v>0.2</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J4" s="1">
         <v>0.8</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>